<commit_message>
Updated code for project
</commit_message>
<xml_diff>
--- a/pandas/tests/io/excel/test_file.xlsx
+++ b/pandas/tests/io/excel/test_file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Numbers</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Test_Column</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -357,13 +372,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H16" sqref="H16:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -371,18 +389,28 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>